<commit_message>
Gdown implemented and working
</commit_message>
<xml_diff>
--- a/RunningStat.xlsx
+++ b/RunningStat.xlsx
@@ -43,9 +43,6 @@
     <t>156.5</t>
   </si>
   <si>
-    <t>14.03.23</t>
-  </si>
-  <si>
     <t>3.15</t>
   </si>
   <si>
@@ -58,9 +55,6 @@
     <t>116</t>
   </si>
   <si>
-    <t>16.03.23</t>
-  </si>
-  <si>
     <t>3.32</t>
   </si>
   <si>
@@ -70,9 +64,6 @@
     <t>05:21:00</t>
   </si>
   <si>
-    <t>21.03.23</t>
-  </si>
-  <si>
     <t>3.08</t>
   </si>
   <si>
@@ -85,9 +76,6 @@
     <t>109.8</t>
   </si>
   <si>
-    <t>22.03.23</t>
-  </si>
-  <si>
     <t>3,07</t>
   </si>
   <si>
@@ -100,7 +88,19 @@
     <t>95,5</t>
   </si>
   <si>
-    <t>24.03.23</t>
+    <t>14.03.2023</t>
+  </si>
+  <si>
+    <t>16.03.2023</t>
+  </si>
+  <si>
+    <t>21.03.2023</t>
+  </si>
+  <si>
+    <t>22.03.2023</t>
+  </si>
+  <si>
+    <t>24.03.2023</t>
   </si>
 </sst>
 </file>
@@ -457,7 +457,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -492,72 +494,72 @@
         <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
         <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>17</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
         <v>19</v>
       </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" t="s">
-        <v>22</v>
-      </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E6" t="s">
         <v>28</v>

</xml_diff>